<commit_message>
Added the ability to test different genotypes
</commit_message>
<xml_diff>
--- a/notebooks/SUOX/input/Li-SUOX-SupplTable-35.xlsx
+++ b/notebooks/SUOX/input/Li-SUOX-SupplTable-35.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rekerl/Documents/Programs/genophenocorr/notebooks/SUOX/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE69769B-11B6-C34A-A9E1-EBE2595BB1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E037781-10BC-8C4F-AE71-86A2BC230CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{7E2479EB-4D84-BF4E-98EC-A88AD1429645}"/>
+    <workbookView xWindow="-28220" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7E2479EB-4D84-BF4E-98EC-A88AD1429645}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -820,9 +820,6 @@
     <t>c.1200C&gt;G;c.650G&gt;A</t>
   </si>
   <si>
-    <t>c.1200C&gt;G;c.1355C&gt;A</t>
-  </si>
-  <si>
     <t>c.352C&gt;T;c.649C&gt;G</t>
   </si>
   <si>
@@ -836,6 +833,9 @@
   </si>
   <si>
     <t>c.205G&gt;C;c.1200C&gt;G</t>
+  </si>
+  <si>
+    <t>c.1200C&gt;G;c.1355G&gt;A</t>
   </si>
 </sst>
 </file>
@@ -919,7 +919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -945,21 +945,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -969,10 +954,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1291,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA615E8F-5427-7149-A25B-270CDB9350AB}">
   <dimension ref="A1:BC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="137" workbookViewId="0">
-      <selection activeCell="P16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="S18" zoomScale="188" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1301,135 +1295,137 @@
     <col min="8" max="8" width="14.1640625" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
     <col min="25" max="25" width="21.1640625" customWidth="1"/>
+    <col min="40" max="40" width="29.6640625" customWidth="1"/>
+    <col min="43" max="43" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14" t="s">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="14"/>
-      <c r="W1" s="10" t="s">
+      <c r="V1" s="9"/>
+      <c r="W1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9" t="s">
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="10" t="s">
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AD1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AE1" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="10" t="s">
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AK1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AL1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AM1" s="10" t="s">
+      <c r="AM1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AN1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="10" t="s">
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AQ1" s="10" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AR1" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="AS1" s="9"/>
-      <c r="AT1" s="9"/>
-      <c r="AU1" s="9"/>
-      <c r="AV1" s="9"/>
-      <c r="AW1" s="9" t="s">
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="AX1" s="9"/>
-      <c r="AY1" s="9"/>
-      <c r="AZ1" s="9"/>
-      <c r="BA1" s="9"/>
-      <c r="BB1" s="9"/>
-      <c r="BC1" s="9"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
     </row>
     <row r="2" spans="1:55" ht="40" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1439,7 +1435,7 @@
       <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="16"/>
+      <c r="M2" s="11"/>
       <c r="N2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1467,7 +1463,7 @@
       <c r="V2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="12"/>
+      <c r="W2" s="13"/>
       <c r="X2" s="5" t="s">
         <v>103</v>
       </c>
@@ -1483,8 +1479,8 @@
       <c r="AB2" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
       <c r="AE2" s="5" t="s">
         <v>106</v>
       </c>
@@ -1497,19 +1493,19 @@
       <c r="AH2" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="15"/>
+      <c r="AN2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AO2" s="10" t="s">
+      <c r="AO2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AP2" s="11"/>
-      <c r="AQ2" s="11"/>
+      <c r="AP2" s="15"/>
+      <c r="AQ2" s="15"/>
       <c r="AR2" s="7" t="s">
         <v>203</v>
       </c>
@@ -1548,49 +1544,49 @@
       </c>
     </row>
     <row r="3" spans="1:55" ht="79" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="18"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="18"/>
-      <c r="AJ3" s="18"/>
-      <c r="AK3" s="18"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="12"/>
-      <c r="AQ3" s="12"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13"/>
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="13"/>
       <c r="AR3" s="8" t="s">
         <v>204</v>
       </c>
@@ -4809,7 +4805,7 @@
         <v>144</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="Z23" s="4" t="s">
         <v>146</v>
@@ -5304,7 +5300,7 @@
         <v>183</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z26" s="4" t="s">
         <v>184</v>
@@ -5630,7 +5626,7 @@
         <v>185</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z28" s="4" t="s">
         <v>186</v>
@@ -5793,7 +5789,7 @@
         <v>185</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z29" s="4" t="s">
         <v>186</v>
@@ -5956,7 +5952,7 @@
         <v>185</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z30" s="4" t="s">
         <v>186</v>
@@ -6561,7 +6557,7 @@
         <v>194</v>
       </c>
       <c r="Y35" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Z35" s="4" t="s">
         <v>195</v>
@@ -6670,7 +6666,7 @@
         <v>144</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Z36" s="4" t="s">
         <v>146</v>
@@ -6781,7 +6777,7 @@
         <v>144</v>
       </c>
       <c r="Y37" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Z37" s="4" t="s">
         <v>146</v>
@@ -6894,7 +6890,7 @@
         <v>196</v>
       </c>
       <c r="Y38" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Z38" s="4" t="s">
         <v>197</v>
@@ -6935,6 +6931,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AP3"/>
+    <mergeCell ref="AQ1:AQ3"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AW1:BC1"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AM1:AM3"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AL1:AL3"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -6947,24 +6961,6 @@
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:T1"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AM1:AM3"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AL1:AL3"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AP1:AP3"/>
-    <mergeCell ref="AQ1:AQ3"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AW1:BC1"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Switch to using ensembl instead of varcode
</commit_message>
<xml_diff>
--- a/notebooks/SUOX/input/Li-SUOX-SupplTable-35.xlsx
+++ b/notebooks/SUOX/input/Li-SUOX-SupplTable-35.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rekerl/Documents/Programs/genophenocorr/notebooks/SUOX/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E037781-10BC-8C4F-AE71-86A2BC230CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE93091-B9BE-734A-9A71-6A19D5C0F1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28220" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7E2479EB-4D84-BF4E-98EC-A88AD1429645}"/>
+    <workbookView xWindow="2600" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{7E2479EB-4D84-BF4E-98EC-A88AD1429645}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -870,12 +870,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -919,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -967,6 +973,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1285,14 +1297,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA615E8F-5427-7149-A25B-270CDB9350AB}">
   <dimension ref="A1:BC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S18" zoomScale="188" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="188" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="31.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
     <col min="25" max="25" width="21.1640625" customWidth="1"/>
     <col min="40" max="40" width="29.6640625" customWidth="1"/>
@@ -1975,13 +1987,13 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -2303,13 +2315,13 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -3279,13 +3291,13 @@
       <c r="F14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -4098,13 +4110,13 @@
       <c r="F19" s="1">
         <v>0.8</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J19" s="1" t="s">
@@ -4754,13 +4766,13 @@
       <c r="F23" s="1">
         <v>0</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J23" s="1" t="s">
@@ -5247,13 +5259,13 @@
       <c r="F26" s="1">
         <v>0.7</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J26" s="1" t="s">
@@ -5575,13 +5587,13 @@
       <c r="F28" s="1">
         <v>12</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J28" s="1" t="s">
@@ -5738,13 +5750,13 @@
       <c r="F29" s="1">
         <v>16</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J29" s="1" t="s">
@@ -5901,13 +5913,13 @@
       <c r="F30" s="1">
         <v>14</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I30" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J30" s="1" t="s">
@@ -6504,13 +6516,13 @@
       <c r="F35" s="1">
         <v>0.5</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I35" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J35" s="1" t="s">
@@ -6615,13 +6627,13 @@
       <c r="F36" s="1">
         <v>0</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H36" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I36" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J36" s="1" t="s">
@@ -6724,13 +6736,13 @@
       <c r="F37" s="1">
         <v>0.1</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H37" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I37" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J37" s="1" t="s">
@@ -6835,13 +6847,13 @@
       <c r="F38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I38" s="18" t="s">
         <v>43</v>
       </c>
       <c r="J38" s="2" t="s">

</xml_diff>